<commit_message>
Updated exporters to support context data
</commit_message>
<xml_diff>
--- a/WorkBot/refactor/data/orders/FingerLakes Farms/FingerLakes Farms_Collegetown_2025-07-25.xlsx
+++ b/WorkBot/refactor/data/orders/FingerLakes Farms/FingerLakes Farms_Collegetown_2025-07-25.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>18.50</t>
+          <t>9.25</t>
         </is>
       </c>
     </row>
@@ -661,6 +661,33 @@
       <c r="E9" t="inlineStr">
         <is>
           <t>80.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>004061</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Natalie's - Honey Tangerine</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>14.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>14.00</t>
         </is>
       </c>
     </row>

</xml_diff>